<commit_message>
Finished Analysis of penalty taker of Pontedera
</commit_message>
<xml_diff>
--- a/coppa/squadre/pontedera/ianesi/Rigori_Ianesi.xlsx
+++ b/coppa/squadre/pontedera/ianesi/Rigori_Ianesi.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Ianesi" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Foglio1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -63,11 +63,11 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,15 +84,30 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -309,9 +324,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="20.38"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -335,52 +347,185 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>1.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>11.0</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>10.0</v>
       </c>
-      <c r="E2" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="H2" s="3"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>1.0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>4.0</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>9.0</v>
       </c>
-      <c r="E3" s="1">
-        <v>26.0</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="3">
+        <v>27.0</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="7"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>